<commit_message>
database python file created, database update and simple_graph update
</commit_message>
<xml_diff>
--- a/teams_2021-2022_stats.xlsx
+++ b/teams_2021-2022_stats.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goeth\Desktop\Projet basket alex\Basketball_lover\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E1CC6C0-6BF1-49D3-85FF-205A451D3F59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A7B2D77-B67D-417F-839A-E2459F0A29BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{086CA7C8-66FA-4EDE-97F0-3770D0E4C9E1}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{086CA7C8-66FA-4EDE-97F0-3770D0E4C9E1}"/>
   </bookViews>
   <sheets>
     <sheet name="team 2021-2022 stats regular" sheetId="2" r:id="rId1"/>
     <sheet name="Feuil1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="DonnéesExternes_1" localSheetId="0" hidden="1">'team 2021-2022 stats regular'!$A$1:$Y$32</definedName>
+    <definedName name="DonnéesExternes_1" localSheetId="0" hidden="1">'team 2021-2022 stats regular'!$A$1:$Z$32</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="588">
   <si>
     <t>Rk,Team,G,MP,FG,FGA,FG%,3P,3PA,3P%,2P,2PA,2P%,FT,FTA,FT%,ORB,DRB,TRB,AST,STL,BLK,TOV,PF,PTS</t>
   </si>
@@ -1716,6 +1716,102 @@
   </si>
   <si>
     <t>Dallas Mavericks</t>
+  </si>
+  <si>
+    <t>Nickname</t>
+  </si>
+  <si>
+    <t>MIN</t>
+  </si>
+  <si>
+    <t>MEM</t>
+  </si>
+  <si>
+    <t>MIL</t>
+  </si>
+  <si>
+    <t>CHA</t>
+  </si>
+  <si>
+    <t>ATL</t>
+  </si>
+  <si>
+    <t>UTA</t>
+  </si>
+  <si>
+    <t>DEN</t>
+  </si>
+  <si>
+    <t>BOS</t>
+  </si>
+  <si>
+    <t>CHI</t>
+  </si>
+  <si>
+    <t>IND</t>
+  </si>
+  <si>
+    <t>SAC</t>
+  </si>
+  <si>
+    <t>MIA</t>
+  </si>
+  <si>
+    <t>PHI</t>
+  </si>
+  <si>
+    <t>HOU</t>
+  </si>
+  <si>
+    <t>TOR</t>
+  </si>
+  <si>
+    <t>WAS</t>
+  </si>
+  <si>
+    <t>DAL</t>
+  </si>
+  <si>
+    <t>CLE</t>
+  </si>
+  <si>
+    <t>POR</t>
+  </si>
+  <si>
+    <t>DET</t>
+  </si>
+  <si>
+    <t>ORL</t>
+  </si>
+  <si>
+    <t>LEA</t>
+  </si>
+  <si>
+    <t>PHX</t>
+  </si>
+  <si>
+    <t>SAS</t>
+  </si>
+  <si>
+    <t>BKN</t>
+  </si>
+  <si>
+    <t>LAL</t>
+  </si>
+  <si>
+    <t>GSW</t>
+  </si>
+  <si>
+    <t>NOP</t>
+  </si>
+  <si>
+    <t>LAC</t>
+  </si>
+  <si>
+    <t>NYK</t>
+  </si>
+  <si>
+    <t>OKC</t>
   </si>
 </sst>
 </file>
@@ -1756,12 +1852,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1851,10 +1946,11 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DonnéesExternes_1" connectionId="1" xr16:uid="{553BAB84-DEC3-45D3-864A-077D497413CA}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="26">
-    <queryTableFields count="25">
+  <queryTableRefresh nextId="27">
+    <queryTableFields count="26">
       <queryTableField id="1" name="Rk" tableColumnId="1"/>
       <queryTableField id="2" name="Team" tableColumnId="2"/>
+      <queryTableField id="26" dataBound="0" tableColumnId="26"/>
       <queryTableField id="3" name="G" tableColumnId="3"/>
       <queryTableField id="4" name="MP" tableColumnId="4"/>
       <queryTableField id="5" name="FG" tableColumnId="5"/>
@@ -1884,11 +1980,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F9CC6422-B176-4392-AA94-99465B811BCC}" name="team_2021_2022_stats_regular" displayName="team_2021_2022_stats_regular" ref="A1:Y32" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:Y32" xr:uid="{F9CC6422-B176-4392-AA94-99465B811BCC}"/>
-  <tableColumns count="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F9CC6422-B176-4392-AA94-99465B811BCC}" name="team_2021_2022_stats_regular" displayName="team_2021_2022_stats_regular" ref="A1:Z32" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:Z32" xr:uid="{F9CC6422-B176-4392-AA94-99465B811BCC}"/>
+  <tableColumns count="26">
     <tableColumn id="1" xr3:uid="{10C23C06-E20D-446F-AFEB-86C71C7A114F}" uniqueName="1" name="Rk" queryTableFieldId="1"/>
     <tableColumn id="2" xr3:uid="{13F820A5-16D2-4835-97DA-B56BE2DE5897}" uniqueName="2" name="Team" queryTableFieldId="2" dataDxfId="22"/>
+    <tableColumn id="26" xr3:uid="{1B395C8E-2CFF-4A2C-9585-942FE87B55FF}" uniqueName="26" name="Nickname" queryTableFieldId="26"/>
     <tableColumn id="3" xr3:uid="{F6CC3844-20D8-4461-8585-25565273960D}" uniqueName="3" name="G" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{8D4A936A-ADA6-4FCE-8B1F-97F8F25EC59A}" uniqueName="4" name="MP" queryTableFieldId="4" dataDxfId="21"/>
     <tableColumn id="5" xr3:uid="{3C50F7D6-AEAE-4B5A-8709-91AE61A546A0}" uniqueName="5" name="FG" queryTableFieldId="5" dataDxfId="20"/>
@@ -2234,41 +2331,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21E31818-8CC7-42EE-9CE7-4DA19C411972}">
-  <dimension ref="A1:Y32"/>
+  <dimension ref="A1:Z32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:26">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -2276,2456 +2374,2552 @@
         <v>33</v>
       </c>
       <c r="C1" t="s">
+        <v>556</v>
+      </c>
+      <c r="D1" t="s">
         <v>34</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>35</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>36</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>37</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>38</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>39</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>40</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>41</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>42</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>43</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>44</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>45</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>46</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>47</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>48</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>49</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>50</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>51</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>52</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>53</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>54</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>55</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:26">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
         <v>540</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="s">
+        <v>557</v>
+      </c>
+      <c r="D2">
         <v>82</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" t="s">
         <v>58</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" t="s">
         <v>59</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" t="s">
         <v>60</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" t="s">
         <v>61</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" t="s">
         <v>62</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" t="s">
         <v>63</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" t="s">
         <v>64</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" t="s">
         <v>65</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" t="s">
         <v>66</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" t="s">
         <v>67</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" t="s">
         <v>68</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="Q2" t="s">
         <v>69</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="R2" t="s">
         <v>70</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="S2" t="s">
         <v>71</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="T2" t="s">
         <v>72</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="U2" t="s">
         <v>73</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="V2" t="s">
         <v>74</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="W2" t="s">
         <v>75</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="X2" t="s">
         <v>76</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="Y2" t="s">
         <v>77</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="Z2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:26">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" t="s">
         <v>541</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="s">
+        <v>558</v>
+      </c>
+      <c r="D3">
         <v>82</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" t="s">
         <v>57</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" t="s">
         <v>79</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" t="s">
         <v>80</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" t="s">
         <v>81</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" t="s">
         <v>82</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" t="s">
         <v>83</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" t="s">
         <v>84</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="L3" t="s">
         <v>85</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="M3" t="s">
         <v>86</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="N3" t="s">
         <v>87</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="O3" t="s">
         <v>88</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="P3" t="s">
         <v>68</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="Q3" t="s">
         <v>89</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="R3" t="s">
         <v>90</v>
       </c>
-      <c r="R3" s="2" t="s">
+      <c r="S3" t="s">
         <v>91</v>
       </c>
-      <c r="S3" s="2" t="s">
+      <c r="T3" t="s">
         <v>92</v>
       </c>
-      <c r="T3" s="2" t="s">
+      <c r="U3" t="s">
         <v>93</v>
       </c>
-      <c r="U3" s="2" t="s">
+      <c r="V3" t="s">
         <v>94</v>
       </c>
-      <c r="V3" s="2" t="s">
+      <c r="W3" t="s">
         <v>95</v>
       </c>
-      <c r="W3" s="2" t="s">
+      <c r="X3" t="s">
         <v>96</v>
       </c>
-      <c r="X3" s="2" t="s">
+      <c r="Y3" t="s">
         <v>97</v>
       </c>
-      <c r="Y3" s="2" t="s">
+      <c r="Z3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:26">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" t="s">
         <v>542</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="s">
+        <v>559</v>
+      </c>
+      <c r="D4">
         <v>82</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" t="s">
         <v>99</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" t="s">
         <v>100</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" t="s">
         <v>101</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" t="s">
         <v>102</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" t="s">
         <v>90</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" t="s">
         <v>103</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="K4" t="s">
         <v>104</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="L4" t="s">
         <v>105</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="M4" t="s">
         <v>106</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="N4" t="s">
         <v>107</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="O4" t="s">
         <v>108</v>
       </c>
-      <c r="O4" s="2" t="s">
+      <c r="P4" t="s">
         <v>109</v>
       </c>
-      <c r="P4" s="2" t="s">
+      <c r="Q4" t="s">
         <v>110</v>
       </c>
-      <c r="Q4" s="2" t="s">
+      <c r="R4" t="s">
         <v>111</v>
       </c>
-      <c r="R4" s="2" t="s">
+      <c r="S4" t="s">
         <v>112</v>
       </c>
-      <c r="S4" s="2" t="s">
+      <c r="T4" t="s">
         <v>113</v>
       </c>
-      <c r="T4" s="2" t="s">
+      <c r="U4" t="s">
         <v>114</v>
       </c>
-      <c r="U4" s="2" t="s">
+      <c r="V4" t="s">
         <v>115</v>
       </c>
-      <c r="V4" s="2" t="s">
+      <c r="W4" t="s">
         <v>116</v>
       </c>
-      <c r="W4" s="2" t="s">
+      <c r="X4" t="s">
         <v>117</v>
       </c>
-      <c r="X4" s="2" t="s">
+      <c r="Y4" t="s">
         <v>118</v>
       </c>
-      <c r="Y4" s="2" t="s">
+      <c r="Z4" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:26">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" t="s">
         <v>120</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="s">
+        <v>560</v>
+      </c>
+      <c r="D5">
         <v>82</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" t="s">
         <v>121</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" t="s">
         <v>122</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" t="s">
         <v>123</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" t="s">
         <v>102</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" t="s">
         <v>124</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="J5" t="s">
         <v>125</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="K5" t="s">
         <v>126</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="L5" t="s">
         <v>127</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="M5" t="s">
         <v>128</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="N5" t="s">
         <v>129</v>
       </c>
-      <c r="N5" s="2" t="s">
+      <c r="O5" t="s">
         <v>130</v>
       </c>
-      <c r="O5" s="2" t="s">
+      <c r="P5" t="s">
         <v>131</v>
       </c>
-      <c r="P5" s="2" t="s">
+      <c r="Q5" t="s">
         <v>132</v>
       </c>
-      <c r="Q5" s="2" t="s">
+      <c r="R5" t="s">
         <v>133</v>
       </c>
-      <c r="R5" s="2" t="s">
+      <c r="S5" t="s">
         <v>134</v>
       </c>
-      <c r="S5" s="2" t="s">
+      <c r="T5" t="s">
         <v>135</v>
       </c>
-      <c r="T5" s="2" t="s">
+      <c r="U5" t="s">
         <v>136</v>
       </c>
-      <c r="U5" s="2" t="s">
+      <c r="V5" t="s">
         <v>137</v>
       </c>
-      <c r="V5" s="2" t="s">
+      <c r="W5" t="s">
         <v>138</v>
       </c>
-      <c r="W5" s="2" t="s">
+      <c r="X5" t="s">
         <v>139</v>
       </c>
-      <c r="X5" s="2" t="s">
+      <c r="Y5" t="s">
         <v>140</v>
       </c>
-      <c r="Y5" s="2" t="s">
+      <c r="Z5" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:26">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" t="s">
         <v>543</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="s">
+        <v>579</v>
+      </c>
+      <c r="D6">
         <v>82</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" t="s">
         <v>142</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" t="s">
         <v>143</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="G6" t="s">
         <v>144</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" t="s">
         <v>145</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" t="s">
         <v>146</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="J6" t="s">
         <v>147</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="K6" t="s">
         <v>148</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="L6" t="s">
         <v>149</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="M6" t="s">
         <v>150</v>
       </c>
-      <c r="M6" s="2" t="s">
+      <c r="N6" t="s">
         <v>151</v>
       </c>
-      <c r="N6" s="2" t="s">
+      <c r="O6" t="s">
         <v>152</v>
       </c>
-      <c r="O6" s="2" t="s">
+      <c r="P6" t="s">
         <v>140</v>
       </c>
-      <c r="P6" s="2" t="s">
+      <c r="Q6" t="s">
         <v>153</v>
       </c>
-      <c r="Q6" s="2" t="s">
+      <c r="R6" t="s">
         <v>94</v>
       </c>
-      <c r="R6" s="2" t="s">
+      <c r="S6" t="s">
         <v>154</v>
       </c>
-      <c r="S6" s="2" t="s">
+      <c r="T6" t="s">
         <v>155</v>
       </c>
-      <c r="T6" s="2" t="s">
+      <c r="U6" t="s">
         <v>156</v>
       </c>
-      <c r="U6" s="2" t="s">
+      <c r="V6" t="s">
         <v>137</v>
       </c>
-      <c r="V6" s="2" t="s">
+      <c r="W6" t="s">
         <v>157</v>
       </c>
-      <c r="W6" s="2" t="s">
+      <c r="X6" t="s">
         <v>158</v>
       </c>
-      <c r="X6" s="2" t="s">
+      <c r="Y6" t="s">
         <v>140</v>
       </c>
-      <c r="Y6" s="2" t="s">
+      <c r="Z6" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:26">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" t="s">
         <v>544</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="s">
+        <v>561</v>
+      </c>
+      <c r="D7">
         <v>82</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" t="s">
         <v>160</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" t="s">
         <v>161</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="G7" t="s">
         <v>162</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" t="s">
         <v>163</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="I7" t="s">
         <v>158</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="J7" t="s">
         <v>164</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="K7" t="s">
         <v>165</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="L7" t="s">
         <v>166</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="M7" t="s">
         <v>167</v>
       </c>
-      <c r="M7" s="2" t="s">
+      <c r="N7" t="s">
         <v>168</v>
       </c>
-      <c r="N7" s="2" t="s">
+      <c r="O7" t="s">
         <v>169</v>
       </c>
-      <c r="O7" s="2" t="s">
+      <c r="P7" t="s">
         <v>170</v>
       </c>
-      <c r="P7" s="2" t="s">
+      <c r="Q7" t="s">
         <v>171</v>
       </c>
-      <c r="Q7" s="2" t="s">
+      <c r="R7" t="s">
         <v>172</v>
       </c>
-      <c r="R7" s="2" t="s">
+      <c r="S7" t="s">
         <v>173</v>
       </c>
-      <c r="S7" s="2" t="s">
+      <c r="T7" t="s">
         <v>174</v>
       </c>
-      <c r="T7" s="2" t="s">
+      <c r="U7" t="s">
         <v>175</v>
       </c>
-      <c r="U7" s="2" t="s">
+      <c r="V7" t="s">
         <v>176</v>
       </c>
-      <c r="V7" s="2" t="s">
+      <c r="W7" t="s">
         <v>177</v>
       </c>
-      <c r="W7" s="2" t="s">
+      <c r="X7" t="s">
         <v>178</v>
       </c>
-      <c r="X7" s="2" t="s">
+      <c r="Y7" t="s">
         <v>179</v>
       </c>
-      <c r="Y7" s="2" t="s">
+      <c r="Z7" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:26">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" t="s">
         <v>545</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="s">
+        <v>562</v>
+      </c>
+      <c r="D8">
         <v>82</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" t="s">
         <v>142</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" t="s">
         <v>181</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="G8" t="s">
         <v>182</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" t="s">
         <v>183</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="I8" t="s">
         <v>184</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="J8" t="s">
         <v>185</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="K8" t="s">
         <v>186</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="L8" t="s">
         <v>93</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="M8" t="s">
         <v>187</v>
       </c>
-      <c r="M8" s="2" t="s">
+      <c r="N8" t="s">
         <v>188</v>
       </c>
-      <c r="N8" s="2" t="s">
+      <c r="O8" t="s">
         <v>189</v>
       </c>
-      <c r="O8" s="2" t="s">
+      <c r="P8" t="s">
         <v>190</v>
       </c>
-      <c r="P8" s="2" t="s">
+      <c r="Q8" t="s">
         <v>191</v>
       </c>
-      <c r="Q8" s="2" t="s">
+      <c r="R8" t="s">
         <v>133</v>
       </c>
-      <c r="R8" s="2" t="s">
+      <c r="S8" t="s">
         <v>192</v>
       </c>
-      <c r="S8" s="2" t="s">
+      <c r="T8" t="s">
         <v>193</v>
       </c>
-      <c r="T8" s="2" t="s">
+      <c r="U8" t="s">
         <v>194</v>
       </c>
-      <c r="U8" s="2" t="s">
+      <c r="V8" t="s">
         <v>176</v>
       </c>
-      <c r="V8" s="2" t="s">
+      <c r="W8" t="s">
         <v>138</v>
       </c>
-      <c r="W8" s="2" t="s">
+      <c r="X8" t="s">
         <v>195</v>
       </c>
-      <c r="X8" s="2" t="s">
+      <c r="Y8" t="s">
         <v>196</v>
       </c>
-      <c r="Y8" s="2" t="s">
+      <c r="Z8" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:26">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" t="s">
         <v>198</v>
       </c>
-      <c r="C9">
+      <c r="C9" t="s">
+        <v>580</v>
+      </c>
+      <c r="D9">
         <v>82</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" t="s">
         <v>199</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" t="s">
         <v>200</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="G9" t="s">
         <v>201</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="H9" t="s">
         <v>202</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="I9" t="s">
         <v>203</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="J9" t="s">
         <v>85</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="K9" t="s">
         <v>204</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="L9" t="s">
         <v>85</v>
       </c>
-      <c r="L9" s="2" t="s">
+      <c r="M9" t="s">
         <v>205</v>
       </c>
-      <c r="M9" s="2" t="s">
+      <c r="N9" t="s">
         <v>206</v>
       </c>
-      <c r="N9" s="2" t="s">
+      <c r="O9" t="s">
         <v>207</v>
       </c>
-      <c r="O9" s="2" t="s">
+      <c r="P9" t="s">
         <v>208</v>
       </c>
-      <c r="P9" s="2" t="s">
+      <c r="Q9" t="s">
         <v>209</v>
       </c>
-      <c r="Q9" s="2" t="s">
+      <c r="R9" t="s">
         <v>210</v>
       </c>
-      <c r="R9" s="2" t="s">
+      <c r="S9" t="s">
         <v>211</v>
       </c>
-      <c r="S9" s="2" t="s">
+      <c r="T9" t="s">
         <v>155</v>
       </c>
-      <c r="T9" s="2" t="s">
+      <c r="U9" t="s">
         <v>212</v>
       </c>
-      <c r="U9" s="2" t="s">
+      <c r="V9" t="s">
         <v>115</v>
       </c>
-      <c r="V9" s="2" t="s">
+      <c r="W9" t="s">
         <v>138</v>
       </c>
-      <c r="W9" s="2" t="s">
+      <c r="X9" t="s">
         <v>213</v>
       </c>
-      <c r="X9" s="2" t="s">
+      <c r="Y9" t="s">
         <v>169</v>
       </c>
-      <c r="Y9" s="2" t="s">
+      <c r="Z9" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:26">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" t="s">
         <v>546</v>
       </c>
-      <c r="C10">
+      <c r="C10" t="s">
+        <v>581</v>
+      </c>
+      <c r="D10">
         <v>82</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" t="s">
         <v>99</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" t="s">
         <v>215</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="G10" t="s">
         <v>216</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="H10" t="s">
         <v>217</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="I10" t="s">
         <v>82</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="J10" t="s">
         <v>218</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="K10" t="s">
         <v>219</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="L10" t="s">
         <v>220</v>
       </c>
-      <c r="L10" s="2" t="s">
+      <c r="M10" t="s">
         <v>221</v>
       </c>
-      <c r="M10" s="2" t="s">
+      <c r="N10" t="s">
         <v>222</v>
       </c>
-      <c r="N10" s="2" t="s">
+      <c r="O10" t="s">
         <v>223</v>
       </c>
-      <c r="O10" s="2" t="s">
+      <c r="P10" t="s">
         <v>224</v>
       </c>
-      <c r="P10" s="2" t="s">
+      <c r="Q10" t="s">
         <v>225</v>
       </c>
-      <c r="Q10" s="2" t="s">
+      <c r="R10" t="s">
         <v>226</v>
       </c>
-      <c r="R10" s="2" t="s">
+      <c r="S10" t="s">
         <v>227</v>
       </c>
-      <c r="S10" s="2" t="s">
+      <c r="T10" t="s">
         <v>228</v>
       </c>
-      <c r="T10" s="2" t="s">
+      <c r="U10" t="s">
         <v>229</v>
       </c>
-      <c r="U10" s="2" t="s">
+      <c r="V10" t="s">
         <v>230</v>
       </c>
-      <c r="V10" s="2" t="s">
+      <c r="W10" t="s">
         <v>231</v>
       </c>
-      <c r="W10" s="2" t="s">
+      <c r="X10" t="s">
         <v>90</v>
       </c>
-      <c r="X10" s="2" t="s">
+      <c r="Y10" t="s">
         <v>208</v>
       </c>
-      <c r="Y10" s="2" t="s">
+      <c r="Z10" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="11" spans="1:25">
+    <row r="11" spans="1:26">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" t="s">
         <v>547</v>
       </c>
-      <c r="C11">
+      <c r="C11" t="s">
+        <v>563</v>
+      </c>
+      <c r="D11">
         <v>82</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" t="s">
         <v>199</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="F11" t="s">
         <v>233</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="G11" t="s">
         <v>234</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="H11" t="s">
         <v>235</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="I11" t="s">
         <v>213</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="J11" t="s">
         <v>236</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="K11" t="s">
         <v>84</v>
       </c>
-      <c r="K11" s="2" t="s">
+      <c r="L11" t="s">
         <v>237</v>
       </c>
-      <c r="L11" s="2" t="s">
+      <c r="M11" t="s">
         <v>238</v>
       </c>
-      <c r="M11" s="2" t="s">
+      <c r="N11" t="s">
         <v>239</v>
       </c>
-      <c r="N11" s="2" t="s">
+      <c r="O11" t="s">
         <v>240</v>
       </c>
-      <c r="O11" s="2" t="s">
+      <c r="P11" t="s">
         <v>241</v>
       </c>
-      <c r="P11" s="2" t="s">
+      <c r="Q11" t="s">
         <v>242</v>
       </c>
-      <c r="Q11" s="2" t="s">
+      <c r="R11" t="s">
         <v>243</v>
       </c>
-      <c r="R11" s="2" t="s">
+      <c r="S11" t="s">
         <v>244</v>
       </c>
-      <c r="S11" s="2" t="s">
+      <c r="T11" t="s">
         <v>245</v>
       </c>
-      <c r="T11" s="2" t="s">
+      <c r="U11" t="s">
         <v>105</v>
       </c>
-      <c r="U11" s="2" t="s">
+      <c r="V11" t="s">
         <v>176</v>
       </c>
-      <c r="V11" s="2" t="s">
+      <c r="W11" t="s">
         <v>246</v>
       </c>
-      <c r="W11" s="2" t="s">
+      <c r="X11" t="s">
         <v>184</v>
       </c>
-      <c r="X11" s="2" t="s">
+      <c r="Y11" t="s">
         <v>247</v>
       </c>
-      <c r="Y11" s="2" t="s">
+      <c r="Z11" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="12" spans="1:25">
+    <row r="12" spans="1:26">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" t="s">
         <v>249</v>
       </c>
-      <c r="C12">
+      <c r="C12" t="s">
+        <v>582</v>
+      </c>
+      <c r="D12">
         <v>82</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" t="s">
         <v>250</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="F12" t="s">
         <v>58</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="G12" t="s">
         <v>251</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="H12" t="s">
         <v>252</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="I12" t="s">
         <v>253</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="J12" t="s">
         <v>254</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="K12" t="s">
         <v>255</v>
       </c>
-      <c r="K12" s="2" t="s">
+      <c r="L12" t="s">
         <v>256</v>
       </c>
-      <c r="L12" s="2" t="s">
+      <c r="M12" t="s">
         <v>257</v>
       </c>
-      <c r="M12" s="2" t="s">
+      <c r="N12" t="s">
         <v>258</v>
       </c>
-      <c r="N12" s="2" t="s">
+      <c r="O12" t="s">
         <v>259</v>
       </c>
-      <c r="O12" s="2" t="s">
+      <c r="P12" t="s">
         <v>260</v>
       </c>
-      <c r="P12" s="2" t="s">
+      <c r="Q12" t="s">
         <v>261</v>
       </c>
-      <c r="Q12" s="2" t="s">
+      <c r="R12" t="s">
         <v>262</v>
       </c>
-      <c r="R12" s="2" t="s">
+      <c r="S12" t="s">
         <v>254</v>
       </c>
-      <c r="S12" s="2" t="s">
+      <c r="T12" t="s">
         <v>174</v>
       </c>
-      <c r="T12" s="2" t="s">
+      <c r="U12" t="s">
         <v>263</v>
       </c>
-      <c r="U12" s="2" t="s">
+      <c r="V12" t="s">
         <v>115</v>
       </c>
-      <c r="V12" s="2" t="s">
+      <c r="W12" t="s">
         <v>264</v>
       </c>
-      <c r="W12" s="2" t="s">
+      <c r="X12" t="s">
         <v>184</v>
       </c>
-      <c r="X12" s="2" t="s">
+      <c r="Y12" t="s">
         <v>265</v>
       </c>
-      <c r="Y12" s="2" t="s">
+      <c r="Z12" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="13" spans="1:25">
+    <row r="13" spans="1:26">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" t="s">
         <v>548</v>
       </c>
-      <c r="C13">
+      <c r="C13" t="s">
+        <v>564</v>
+      </c>
+      <c r="D13">
         <v>82</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" t="s">
         <v>267</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="F13" t="s">
         <v>268</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="G13" t="s">
         <v>269</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="H13" t="s">
         <v>270</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="I13" t="s">
         <v>96</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="J13" t="s">
         <v>271</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="K13" t="s">
         <v>272</v>
       </c>
-      <c r="K13" s="2" t="s">
+      <c r="L13" t="s">
         <v>273</v>
       </c>
-      <c r="L13" s="2" t="s">
+      <c r="M13" t="s">
         <v>274</v>
       </c>
-      <c r="M13" s="2" t="s">
+      <c r="N13" t="s">
         <v>275</v>
       </c>
-      <c r="N13" s="2" t="s">
+      <c r="O13" t="s">
         <v>88</v>
       </c>
-      <c r="O13" s="2" t="s">
+      <c r="P13" t="s">
         <v>276</v>
       </c>
-      <c r="P13" s="2" t="s">
+      <c r="Q13" t="s">
         <v>277</v>
       </c>
-      <c r="Q13" s="2" t="s">
+      <c r="R13" t="s">
         <v>278</v>
       </c>
-      <c r="R13" s="2" t="s">
+      <c r="S13" t="s">
         <v>154</v>
       </c>
-      <c r="S13" s="2" t="s">
+      <c r="T13" t="s">
         <v>279</v>
       </c>
-      <c r="T13" s="2" t="s">
+      <c r="U13" t="s">
         <v>280</v>
       </c>
-      <c r="U13" s="2" t="s">
+      <c r="V13" t="s">
         <v>176</v>
       </c>
-      <c r="V13" s="2" t="s">
+      <c r="W13" t="s">
         <v>281</v>
       </c>
-      <c r="W13" s="2" t="s">
+      <c r="X13" t="s">
         <v>282</v>
       </c>
-      <c r="X13" s="2" t="s">
+      <c r="Y13" t="s">
         <v>283</v>
       </c>
-      <c r="Y13" s="2" t="s">
+      <c r="Z13" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="14" spans="1:25">
+    <row r="14" spans="1:26">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" t="s">
         <v>549</v>
       </c>
-      <c r="C14">
+      <c r="C14" t="s">
+        <v>565</v>
+      </c>
+      <c r="D14">
         <v>82</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" t="s">
         <v>142</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="F14" t="s">
         <v>233</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="G14" t="s">
         <v>285</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="H14" t="s">
         <v>286</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="I14" t="s">
         <v>287</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="J14" t="s">
         <v>127</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="K14" t="s">
         <v>288</v>
       </c>
-      <c r="K14" s="2" t="s">
+      <c r="L14" t="s">
         <v>289</v>
       </c>
-      <c r="L14" s="2" t="s">
+      <c r="M14" t="s">
         <v>290</v>
       </c>
-      <c r="M14" s="2" t="s">
+      <c r="N14" t="s">
         <v>291</v>
       </c>
-      <c r="N14" s="2" t="s">
+      <c r="O14" t="s">
         <v>223</v>
       </c>
-      <c r="O14" s="2" t="s">
+      <c r="P14" t="s">
         <v>292</v>
       </c>
-      <c r="P14" s="2" t="s">
+      <c r="Q14" t="s">
         <v>293</v>
       </c>
-      <c r="Q14" s="2" t="s">
+      <c r="R14" t="s">
         <v>294</v>
       </c>
-      <c r="R14" s="2" t="s">
+      <c r="S14" t="s">
         <v>134</v>
       </c>
-      <c r="S14" s="2" t="s">
+      <c r="T14" t="s">
         <v>295</v>
       </c>
-      <c r="T14" s="2" t="s">
+      <c r="U14" t="s">
         <v>114</v>
       </c>
-      <c r="U14" s="2" t="s">
+      <c r="V14" t="s">
         <v>230</v>
       </c>
-      <c r="V14" s="2" t="s">
+      <c r="W14" t="s">
         <v>296</v>
       </c>
-      <c r="W14" s="2" t="s">
+      <c r="X14" t="s">
         <v>297</v>
       </c>
-      <c r="X14" s="2" t="s">
+      <c r="Y14" t="s">
         <v>298</v>
       </c>
-      <c r="Y14" s="2" t="s">
+      <c r="Z14" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:26">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" t="s">
         <v>300</v>
       </c>
-      <c r="C15">
+      <c r="C15" t="s">
+        <v>566</v>
+      </c>
+      <c r="D15">
         <v>82</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" t="s">
         <v>121</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="F15" t="s">
         <v>301</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="G15" t="s">
         <v>302</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="H15" t="s">
         <v>303</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="I15" t="s">
         <v>304</v>
       </c>
-      <c r="I15" s="2" t="s">
+      <c r="J15" t="s">
         <v>305</v>
       </c>
-      <c r="J15" s="2" t="s">
+      <c r="K15" t="s">
         <v>306</v>
       </c>
-      <c r="K15" s="2" t="s">
+      <c r="L15" t="s">
         <v>307</v>
       </c>
-      <c r="L15" s="2" t="s">
+      <c r="M15" t="s">
         <v>308</v>
       </c>
-      <c r="M15" s="2" t="s">
+      <c r="N15" t="s">
         <v>309</v>
       </c>
-      <c r="N15" s="2" t="s">
+      <c r="O15" t="s">
         <v>310</v>
       </c>
-      <c r="O15" s="2" t="s">
+      <c r="P15" t="s">
         <v>131</v>
       </c>
-      <c r="P15" s="2" t="s">
+      <c r="Q15" t="s">
         <v>311</v>
       </c>
-      <c r="Q15" s="2" t="s">
+      <c r="R15" t="s">
         <v>203</v>
       </c>
-      <c r="R15" s="2" t="s">
+      <c r="S15" t="s">
         <v>312</v>
       </c>
-      <c r="S15" s="2" t="s">
+      <c r="T15" t="s">
         <v>313</v>
       </c>
-      <c r="T15" s="2" t="s">
+      <c r="U15" t="s">
         <v>314</v>
       </c>
-      <c r="U15" s="2" t="s">
+      <c r="V15" t="s">
         <v>230</v>
       </c>
-      <c r="V15" s="2" t="s">
+      <c r="W15" t="s">
         <v>75</v>
       </c>
-      <c r="W15" s="2" t="s">
+      <c r="X15" t="s">
         <v>315</v>
       </c>
-      <c r="X15" s="2" t="s">
+      <c r="Y15" t="s">
         <v>208</v>
       </c>
-      <c r="Y15" s="2" t="s">
+      <c r="Z15" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="16" spans="1:25">
+    <row r="16" spans="1:26">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" t="s">
         <v>550</v>
       </c>
-      <c r="C16">
+      <c r="C16" t="s">
+        <v>583</v>
+      </c>
+      <c r="D16">
         <v>82</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="E16" t="s">
         <v>142</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="F16" t="s">
         <v>317</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="G16" t="s">
         <v>318</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="H16" t="s">
         <v>252</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="I16" t="s">
         <v>76</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="J16" t="s">
         <v>319</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="K16" t="s">
         <v>148</v>
       </c>
-      <c r="K16" s="2" t="s">
+      <c r="L16" t="s">
         <v>320</v>
       </c>
-      <c r="L16" s="2" t="s">
+      <c r="M16" t="s">
         <v>321</v>
       </c>
-      <c r="M16" s="2" t="s">
+      <c r="N16" t="s">
         <v>322</v>
       </c>
-      <c r="N16" s="2" t="s">
+      <c r="O16" t="s">
         <v>323</v>
       </c>
-      <c r="O16" s="2" t="s">
+      <c r="P16" t="s">
         <v>324</v>
       </c>
-      <c r="P16" s="2" t="s">
+      <c r="Q16" t="s">
         <v>325</v>
       </c>
-      <c r="Q16" s="2" t="s">
+      <c r="R16" t="s">
         <v>94</v>
       </c>
-      <c r="R16" s="2" t="s">
+      <c r="S16" t="s">
         <v>326</v>
       </c>
-      <c r="S16" s="2" t="s">
+      <c r="T16" t="s">
         <v>327</v>
       </c>
-      <c r="T16" s="2" t="s">
+      <c r="U16" t="s">
         <v>328</v>
       </c>
-      <c r="U16" s="2" t="s">
+      <c r="V16" t="s">
         <v>74</v>
       </c>
-      <c r="V16" s="2" t="s">
+      <c r="W16" t="s">
         <v>329</v>
       </c>
-      <c r="W16" s="2" t="s">
+      <c r="X16" t="s">
         <v>330</v>
       </c>
-      <c r="X16" s="2" t="s">
+      <c r="Y16" t="s">
         <v>241</v>
       </c>
-      <c r="Y16" s="2" t="s">
+      <c r="Z16" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="17" spans="1:25">
+    <row r="17" spans="1:26">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" t="s">
         <v>332</v>
       </c>
-      <c r="C17">
+      <c r="C17" t="s">
+        <v>567</v>
+      </c>
+      <c r="D17">
         <v>82</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="E17" t="s">
         <v>199</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="F17" t="s">
         <v>317</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="G17" t="s">
         <v>333</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="H17" t="s">
         <v>334</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="I17" t="s">
         <v>335</v>
       </c>
-      <c r="I17" s="2" t="s">
+      <c r="J17" t="s">
         <v>336</v>
       </c>
-      <c r="J17" s="2" t="s">
+      <c r="K17" t="s">
         <v>306</v>
       </c>
-      <c r="K17" s="2" t="s">
+      <c r="L17" t="s">
         <v>337</v>
       </c>
-      <c r="L17" s="2" t="s">
+      <c r="M17" t="s">
         <v>338</v>
       </c>
-      <c r="M17" s="2" t="s">
+      <c r="N17" t="s">
         <v>339</v>
       </c>
-      <c r="N17" s="2" t="s">
+      <c r="O17" t="s">
         <v>189</v>
       </c>
-      <c r="O17" s="2" t="s">
+      <c r="P17" t="s">
         <v>340</v>
       </c>
-      <c r="P17" s="2" t="s">
+      <c r="Q17" t="s">
         <v>311</v>
       </c>
-      <c r="Q17" s="2" t="s">
+      <c r="R17" t="s">
         <v>341</v>
       </c>
-      <c r="R17" s="2" t="s">
+      <c r="S17" t="s">
         <v>342</v>
       </c>
-      <c r="S17" s="2" t="s">
+      <c r="T17" t="s">
         <v>343</v>
       </c>
-      <c r="T17" s="2" t="s">
+      <c r="U17" t="s">
         <v>344</v>
       </c>
-      <c r="U17" s="2" t="s">
+      <c r="V17" t="s">
         <v>176</v>
       </c>
-      <c r="V17" s="2" t="s">
+      <c r="W17" t="s">
         <v>329</v>
       </c>
-      <c r="W17" s="2" t="s">
+      <c r="X17" t="s">
         <v>90</v>
       </c>
-      <c r="X17" s="2" t="s">
+      <c r="Y17" t="s">
         <v>196</v>
       </c>
-      <c r="Y17" s="2" t="s">
+      <c r="Z17" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="18" spans="1:25">
+    <row r="18" spans="1:26">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" t="s">
         <v>551</v>
       </c>
-      <c r="C18">
+      <c r="C18" t="s">
+        <v>568</v>
+      </c>
+      <c r="D18">
         <v>82</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="E18" t="s">
         <v>346</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="F18" t="s">
         <v>347</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="G18" t="s">
         <v>348</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="H18" t="s">
         <v>202</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="I18" t="s">
         <v>282</v>
       </c>
-      <c r="I18" s="2" t="s">
+      <c r="J18" t="s">
         <v>349</v>
       </c>
-      <c r="J18" s="2" t="s">
+      <c r="K18" t="s">
         <v>350</v>
       </c>
-      <c r="K18" s="2" t="s">
+      <c r="L18" t="s">
         <v>93</v>
       </c>
-      <c r="L18" s="2" t="s">
+      <c r="M18" t="s">
         <v>351</v>
       </c>
-      <c r="M18" s="2" t="s">
+      <c r="N18" t="s">
         <v>168</v>
       </c>
-      <c r="N18" s="2" t="s">
+      <c r="O18" t="s">
         <v>352</v>
       </c>
-      <c r="O18" s="2" t="s">
+      <c r="P18" t="s">
         <v>131</v>
       </c>
-      <c r="P18" s="2" t="s">
+      <c r="Q18" t="s">
         <v>353</v>
       </c>
-      <c r="Q18" s="2" t="s">
+      <c r="R18" t="s">
         <v>94</v>
       </c>
-      <c r="R18" s="2" t="s">
+      <c r="S18" t="s">
         <v>173</v>
       </c>
-      <c r="S18" s="2" t="s">
+      <c r="T18" t="s">
         <v>143</v>
       </c>
-      <c r="T18" s="2" t="s">
+      <c r="U18" t="s">
         <v>354</v>
       </c>
-      <c r="U18" s="2" t="s">
+      <c r="V18" t="s">
         <v>355</v>
       </c>
-      <c r="V18" s="2" t="s">
+      <c r="W18" t="s">
         <v>356</v>
       </c>
-      <c r="W18" s="2" t="s">
+      <c r="X18" t="s">
         <v>357</v>
       </c>
-      <c r="X18" s="2" t="s">
+      <c r="Y18" t="s">
         <v>358</v>
       </c>
-      <c r="Y18" s="2" t="s">
+      <c r="Z18" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="19" spans="1:25">
+    <row r="19" spans="1:26">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" t="s">
         <v>552</v>
       </c>
-      <c r="C19">
+      <c r="C19" t="s">
+        <v>569</v>
+      </c>
+      <c r="D19">
         <v>82</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="E19" t="s">
         <v>199</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="F19" t="s">
         <v>319</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="G19" t="s">
         <v>360</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="H19" t="s">
         <v>270</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="I19" t="s">
         <v>146</v>
       </c>
-      <c r="I19" s="2" t="s">
+      <c r="J19" t="s">
         <v>361</v>
       </c>
-      <c r="J19" s="2" t="s">
+      <c r="K19" t="s">
         <v>148</v>
       </c>
-      <c r="K19" s="2" t="s">
+      <c r="L19" t="s">
         <v>105</v>
       </c>
-      <c r="L19" s="2" t="s">
+      <c r="M19" t="s">
         <v>362</v>
       </c>
-      <c r="M19" s="2" t="s">
+      <c r="N19" t="s">
         <v>206</v>
       </c>
-      <c r="N19" s="2" t="s">
+      <c r="O19" t="s">
         <v>363</v>
       </c>
-      <c r="O19" s="2" t="s">
+      <c r="P19" t="s">
         <v>364</v>
       </c>
-      <c r="P19" s="2" t="s">
+      <c r="Q19" t="s">
         <v>365</v>
       </c>
-      <c r="Q19" s="2" t="s">
+      <c r="R19" t="s">
         <v>366</v>
       </c>
-      <c r="R19" s="2" t="s">
+      <c r="S19" t="s">
         <v>367</v>
       </c>
-      <c r="S19" s="2" t="s">
+      <c r="T19" t="s">
         <v>295</v>
       </c>
-      <c r="T19" s="2" t="s">
+      <c r="U19" t="s">
         <v>344</v>
       </c>
-      <c r="U19" s="2" t="s">
+      <c r="V19" t="s">
         <v>368</v>
       </c>
-      <c r="V19" s="2" t="s">
+      <c r="W19" t="s">
         <v>369</v>
       </c>
-      <c r="W19" s="2" t="s">
+      <c r="X19" t="s">
         <v>370</v>
       </c>
-      <c r="X19" s="2" t="s">
+      <c r="Y19" t="s">
         <v>371</v>
       </c>
-      <c r="Y19" s="2" t="s">
+      <c r="Z19" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="20" spans="1:25">
+    <row r="20" spans="1:26">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" t="s">
         <v>373</v>
       </c>
-      <c r="C20">
+      <c r="C20" t="s">
+        <v>570</v>
+      </c>
+      <c r="D20">
         <v>82</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="E20" t="s">
         <v>99</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="F20" t="s">
         <v>319</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="G20" t="s">
         <v>318</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="H20" t="s">
         <v>374</v>
       </c>
-      <c r="H20" s="2" t="s">
+      <c r="I20" t="s">
         <v>375</v>
       </c>
-      <c r="I20" s="2" t="s">
+      <c r="J20" t="s">
         <v>376</v>
       </c>
-      <c r="J20" s="2" t="s">
+      <c r="K20" t="s">
         <v>377</v>
       </c>
-      <c r="K20" s="2" t="s">
+      <c r="L20" t="s">
         <v>378</v>
       </c>
-      <c r="L20" s="2" t="s">
+      <c r="M20" t="s">
         <v>379</v>
       </c>
-      <c r="M20" s="2" t="s">
+      <c r="N20" t="s">
         <v>380</v>
       </c>
-      <c r="N20" s="2" t="s">
+      <c r="O20" t="s">
         <v>223</v>
       </c>
-      <c r="O20" s="2" t="s">
+      <c r="P20" t="s">
         <v>381</v>
       </c>
-      <c r="P20" s="2" t="s">
+      <c r="Q20" t="s">
         <v>382</v>
       </c>
-      <c r="Q20" s="2" t="s">
+      <c r="R20" t="s">
         <v>341</v>
       </c>
-      <c r="R20" s="2" t="s">
+      <c r="S20" t="s">
         <v>383</v>
       </c>
-      <c r="S20" s="2" t="s">
+      <c r="T20" t="s">
         <v>215</v>
       </c>
-      <c r="T20" s="2" t="s">
+      <c r="U20" t="s">
         <v>384</v>
       </c>
-      <c r="U20" s="2" t="s">
+      <c r="V20" t="s">
         <v>385</v>
       </c>
-      <c r="V20" s="2" t="s">
+      <c r="W20" t="s">
         <v>386</v>
       </c>
-      <c r="W20" s="2" t="s">
+      <c r="X20" t="s">
         <v>387</v>
       </c>
-      <c r="X20" s="2" t="s">
+      <c r="Y20" t="s">
         <v>388</v>
       </c>
-      <c r="Y20" s="2" t="s">
+      <c r="Z20" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="21" spans="1:25">
+    <row r="21" spans="1:26">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" t="s">
         <v>553</v>
       </c>
-      <c r="C21">
+      <c r="C21" t="s">
+        <v>571</v>
+      </c>
+      <c r="D21">
         <v>82</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="E21" t="s">
         <v>346</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="F21" t="s">
         <v>181</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="G21" t="s">
         <v>390</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="H21" t="s">
         <v>391</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="I21" t="s">
         <v>178</v>
       </c>
-      <c r="I21" s="2" t="s">
+      <c r="J21" t="s">
         <v>392</v>
       </c>
-      <c r="J21" s="2" t="s">
+      <c r="K21" t="s">
         <v>377</v>
       </c>
-      <c r="K21" s="2" t="s">
+      <c r="L21" t="s">
         <v>393</v>
       </c>
-      <c r="L21" s="2" t="s">
+      <c r="M21" t="s">
         <v>394</v>
       </c>
-      <c r="M21" s="2" t="s">
+      <c r="N21" t="s">
         <v>395</v>
       </c>
-      <c r="N21" s="2" t="s">
+      <c r="O21" t="s">
         <v>396</v>
       </c>
-      <c r="O21" s="2" t="s">
+      <c r="P21" t="s">
         <v>397</v>
       </c>
-      <c r="P21" s="2" t="s">
+      <c r="Q21" t="s">
         <v>398</v>
       </c>
-      <c r="Q21" s="2" t="s">
+      <c r="R21" t="s">
         <v>117</v>
       </c>
-      <c r="R21" s="2" t="s">
+      <c r="S21" t="s">
         <v>85</v>
       </c>
-      <c r="S21" s="2" t="s">
+      <c r="T21" t="s">
         <v>155</v>
       </c>
-      <c r="T21" s="2" t="s">
+      <c r="U21" t="s">
         <v>399</v>
       </c>
-      <c r="U21" s="2" t="s">
+      <c r="V21" t="s">
         <v>400</v>
       </c>
-      <c r="V21" s="2" t="s">
+      <c r="W21" t="s">
         <v>401</v>
       </c>
-      <c r="W21" s="2" t="s">
+      <c r="X21" t="s">
         <v>370</v>
       </c>
-      <c r="X21" s="2" t="s">
+      <c r="Y21" t="s">
         <v>363</v>
       </c>
-      <c r="Y21" s="2" t="s">
+      <c r="Z21" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="22" spans="1:25">
+    <row r="22" spans="1:26">
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" t="s">
         <v>554</v>
       </c>
-      <c r="C22">
+      <c r="C22" t="s">
+        <v>584</v>
+      </c>
+      <c r="D22">
         <v>82</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="E22" t="s">
         <v>99</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="F22" t="s">
         <v>403</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="G22" t="s">
         <v>404</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="H22" t="s">
         <v>60</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="I22" t="s">
         <v>287</v>
       </c>
-      <c r="I22" s="2" t="s">
+      <c r="J22" t="s">
         <v>149</v>
       </c>
-      <c r="J22" s="2" t="s">
+      <c r="K22" t="s">
         <v>405</v>
       </c>
-      <c r="K22" s="2" t="s">
+      <c r="L22" t="s">
         <v>406</v>
       </c>
-      <c r="L22" s="2" t="s">
+      <c r="M22" t="s">
         <v>407</v>
       </c>
-      <c r="M22" s="2" t="s">
+      <c r="N22" t="s">
         <v>408</v>
       </c>
-      <c r="N22" s="2" t="s">
+      <c r="O22" t="s">
         <v>409</v>
       </c>
-      <c r="O22" s="2" t="s">
+      <c r="P22" t="s">
         <v>410</v>
       </c>
-      <c r="P22" s="2" t="s">
+      <c r="Q22" t="s">
         <v>411</v>
       </c>
-      <c r="Q22" s="2" t="s">
+      <c r="R22" t="s">
         <v>253</v>
       </c>
-      <c r="R22" s="2" t="s">
+      <c r="S22" t="s">
         <v>336</v>
       </c>
-      <c r="S22" s="2" t="s">
+      <c r="T22" t="s">
         <v>412</v>
       </c>
-      <c r="T22" s="2" t="s">
+      <c r="U22" t="s">
         <v>413</v>
       </c>
-      <c r="U22" s="2" t="s">
+      <c r="V22" t="s">
         <v>414</v>
       </c>
-      <c r="V22" s="2" t="s">
+      <c r="W22" t="s">
         <v>116</v>
       </c>
-      <c r="W22" s="2" t="s">
+      <c r="X22" t="s">
         <v>90</v>
       </c>
-      <c r="X22" s="2" t="s">
+      <c r="Y22" t="s">
         <v>415</v>
       </c>
-      <c r="Y22" s="2" t="s">
+      <c r="Z22" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="23" spans="1:25">
+    <row r="23" spans="1:26">
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" t="s">
         <v>417</v>
       </c>
-      <c r="C23">
+      <c r="C23" t="s">
+        <v>572</v>
+      </c>
+      <c r="D23">
         <v>82</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="E23" t="s">
         <v>418</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="F23" t="s">
         <v>181</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="G23" t="s">
         <v>419</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="H23" t="s">
         <v>420</v>
       </c>
-      <c r="H23" s="2" t="s">
+      <c r="I23" t="s">
         <v>278</v>
       </c>
-      <c r="I23" s="2" t="s">
+      <c r="J23" t="s">
         <v>421</v>
       </c>
-      <c r="J23" s="2" t="s">
+      <c r="K23" t="s">
         <v>422</v>
       </c>
-      <c r="K23" s="2" t="s">
+      <c r="L23" t="s">
         <v>423</v>
       </c>
-      <c r="L23" s="2" t="s">
+      <c r="M23" t="s">
         <v>424</v>
       </c>
-      <c r="M23" s="2" t="s">
+      <c r="N23" t="s">
         <v>380</v>
       </c>
-      <c r="N23" s="2" t="s">
+      <c r="O23" t="s">
         <v>88</v>
       </c>
-      <c r="O23" s="2" t="s">
+      <c r="P23" t="s">
         <v>224</v>
       </c>
-      <c r="P23" s="2" t="s">
+      <c r="Q23" t="s">
         <v>425</v>
       </c>
-      <c r="Q23" s="2" t="s">
+      <c r="R23" t="s">
         <v>400</v>
       </c>
-      <c r="R23" s="2" t="s">
+      <c r="S23" t="s">
         <v>227</v>
       </c>
-      <c r="S23" s="2" t="s">
+      <c r="T23" t="s">
         <v>426</v>
       </c>
-      <c r="T23" s="2" t="s">
+      <c r="U23" t="s">
         <v>413</v>
       </c>
-      <c r="U23" s="2" t="s">
+      <c r="V23" t="s">
         <v>427</v>
       </c>
-      <c r="V23" s="2" t="s">
+      <c r="W23" t="s">
         <v>428</v>
       </c>
-      <c r="W23" s="2" t="s">
+      <c r="X23" t="s">
         <v>429</v>
       </c>
-      <c r="X23" s="2" t="s">
+      <c r="Y23" t="s">
         <v>298</v>
       </c>
-      <c r="Y23" s="2" t="s">
+      <c r="Z23" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="24" spans="1:25">
+    <row r="24" spans="1:26">
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" t="s">
         <v>431</v>
       </c>
-      <c r="C24">
+      <c r="C24" t="s">
+        <v>585</v>
+      </c>
+      <c r="D24">
         <v>82</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="E24" t="s">
         <v>57</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="F24" t="s">
         <v>432</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="G24" t="s">
         <v>269</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="H24" t="s">
         <v>433</v>
       </c>
-      <c r="H24" s="2" t="s">
+      <c r="I24" t="s">
         <v>297</v>
       </c>
-      <c r="I24" s="2" t="s">
+      <c r="J24" t="s">
         <v>392</v>
       </c>
-      <c r="J24" s="2" t="s">
+      <c r="K24" t="s">
         <v>165</v>
       </c>
-      <c r="K24" s="2" t="s">
+      <c r="L24" t="s">
         <v>434</v>
       </c>
-      <c r="L24" s="2" t="s">
+      <c r="M24" t="s">
         <v>128</v>
       </c>
-      <c r="M24" s="2" t="s">
+      <c r="N24" t="s">
         <v>435</v>
       </c>
-      <c r="N24" s="2" t="s">
+      <c r="O24" t="s">
         <v>436</v>
       </c>
-      <c r="O24" s="2" t="s">
+      <c r="P24" t="s">
         <v>363</v>
       </c>
-      <c r="P24" s="2" t="s">
+      <c r="Q24" t="s">
         <v>437</v>
       </c>
-      <c r="Q24" s="2" t="s">
+      <c r="R24" t="s">
         <v>438</v>
       </c>
-      <c r="R24" s="2" t="s">
+      <c r="S24" t="s">
         <v>244</v>
       </c>
-      <c r="S24" s="2" t="s">
+      <c r="T24" t="s">
         <v>174</v>
       </c>
-      <c r="T24" s="2" t="s">
+      <c r="U24" t="s">
         <v>263</v>
       </c>
-      <c r="U24" s="2" t="s">
+      <c r="V24" t="s">
         <v>355</v>
       </c>
-      <c r="V24" s="2" t="s">
+      <c r="W24" t="s">
         <v>428</v>
       </c>
-      <c r="W24" s="2" t="s">
+      <c r="X24" t="s">
         <v>439</v>
       </c>
-      <c r="X24" s="2" t="s">
+      <c r="Y24" t="s">
         <v>440</v>
       </c>
-      <c r="Y24" s="2" t="s">
+      <c r="Z24" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="25" spans="1:25">
+    <row r="25" spans="1:26">
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" t="s">
         <v>555</v>
       </c>
-      <c r="C25">
+      <c r="C25" t="s">
+        <v>573</v>
+      </c>
+      <c r="D25">
         <v>82</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="E25" t="s">
         <v>99</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="F25" t="s">
         <v>442</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="G25" t="s">
         <v>443</v>
       </c>
-      <c r="G25" s="2" t="s">
+      <c r="H25" t="s">
         <v>81</v>
       </c>
-      <c r="H25" s="2" t="s">
+      <c r="I25" t="s">
         <v>429</v>
       </c>
-      <c r="I25" s="2" t="s">
+      <c r="J25" t="s">
         <v>444</v>
       </c>
-      <c r="J25" s="2" t="s">
+      <c r="K25" t="s">
         <v>445</v>
       </c>
-      <c r="K25" s="2" t="s">
+      <c r="L25" t="s">
         <v>320</v>
       </c>
-      <c r="L25" s="2" t="s">
+      <c r="M25" t="s">
         <v>446</v>
       </c>
-      <c r="M25" s="2" t="s">
+      <c r="N25" t="s">
         <v>447</v>
       </c>
-      <c r="N25" s="2" t="s">
+      <c r="O25" t="s">
         <v>310</v>
       </c>
-      <c r="O25" s="2" t="s">
+      <c r="P25" t="s">
         <v>448</v>
       </c>
-      <c r="P25" s="2" t="s">
+      <c r="Q25" t="s">
         <v>449</v>
       </c>
-      <c r="Q25" s="2" t="s">
+      <c r="R25" t="s">
         <v>450</v>
       </c>
-      <c r="R25" s="2" t="s">
+      <c r="S25" t="s">
         <v>367</v>
       </c>
-      <c r="S25" s="2" t="s">
+      <c r="T25" t="s">
         <v>451</v>
       </c>
-      <c r="T25" s="2" t="s">
+      <c r="U25" t="s">
         <v>190</v>
       </c>
-      <c r="U25" s="2" t="s">
+      <c r="V25" t="s">
         <v>452</v>
       </c>
-      <c r="V25" s="2" t="s">
+      <c r="W25" t="s">
         <v>116</v>
       </c>
-      <c r="W25" s="2" t="s">
+      <c r="X25" t="s">
         <v>370</v>
       </c>
-      <c r="X25" s="2" t="s">
+      <c r="Y25" t="s">
         <v>415</v>
       </c>
-      <c r="Y25" s="2" t="s">
+      <c r="Z25" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="26" spans="1:25">
+    <row r="26" spans="1:26">
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" t="s">
         <v>454</v>
       </c>
-      <c r="C26">
+      <c r="C26" t="s">
+        <v>574</v>
+      </c>
+      <c r="D26">
         <v>82</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="E26" t="s">
         <v>142</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="F26" t="s">
         <v>455</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="G26" t="s">
         <v>456</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="H26" t="s">
         <v>252</v>
       </c>
-      <c r="H26" s="2" t="s">
+      <c r="I26" t="s">
         <v>146</v>
       </c>
-      <c r="I26" s="2" t="s">
+      <c r="J26" t="s">
         <v>457</v>
       </c>
-      <c r="J26" s="2" t="s">
+      <c r="K26" t="s">
         <v>458</v>
       </c>
-      <c r="K26" s="2" t="s">
+      <c r="L26" t="s">
         <v>136</v>
       </c>
-      <c r="L26" s="2" t="s">
+      <c r="M26" t="s">
         <v>459</v>
       </c>
-      <c r="M26" s="2" t="s">
+      <c r="N26" t="s">
         <v>309</v>
       </c>
-      <c r="N26" s="2" t="s">
+      <c r="O26" t="s">
         <v>259</v>
       </c>
-      <c r="O26" s="2" t="s">
+      <c r="P26" t="s">
         <v>399</v>
       </c>
-      <c r="P26" s="2" t="s">
+      <c r="Q26" t="s">
         <v>460</v>
       </c>
-      <c r="Q26" s="2" t="s">
+      <c r="R26" t="s">
         <v>111</v>
       </c>
-      <c r="R26" s="2" t="s">
+      <c r="S26" t="s">
         <v>461</v>
       </c>
-      <c r="S26" s="2" t="s">
+      <c r="T26" t="s">
         <v>72</v>
       </c>
-      <c r="T26" s="2" t="s">
+      <c r="U26" t="s">
         <v>462</v>
       </c>
-      <c r="U26" s="2" t="s">
+      <c r="V26" t="s">
         <v>230</v>
       </c>
-      <c r="V26" s="2" t="s">
+      <c r="W26" t="s">
         <v>177</v>
       </c>
-      <c r="W26" s="2" t="s">
+      <c r="X26" t="s">
         <v>315</v>
       </c>
-      <c r="X26" s="2" t="s">
+      <c r="Y26" t="s">
         <v>223</v>
       </c>
-      <c r="Y26" s="2" t="s">
+      <c r="Z26" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="27" spans="1:25">
+    <row r="27" spans="1:26">
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" t="s">
         <v>464</v>
       </c>
-      <c r="C27">
+      <c r="C27" t="s">
+        <v>586</v>
+      </c>
+      <c r="D27">
         <v>82</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="E27" t="s">
         <v>57</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="F27" t="s">
         <v>465</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="G27" t="s">
         <v>182</v>
       </c>
-      <c r="G27" s="2" t="s">
+      <c r="H27" t="s">
         <v>466</v>
       </c>
-      <c r="H27" s="2" t="s">
+      <c r="I27" t="s">
         <v>96</v>
       </c>
-      <c r="I27" s="2" t="s">
+      <c r="J27" t="s">
         <v>467</v>
       </c>
-      <c r="J27" s="2" t="s">
+      <c r="K27" t="s">
         <v>468</v>
       </c>
-      <c r="K27" s="2" t="s">
+      <c r="L27" t="s">
         <v>381</v>
       </c>
-      <c r="L27" s="2" t="s">
+      <c r="M27" t="s">
         <v>469</v>
       </c>
-      <c r="M27" s="2" t="s">
+      <c r="N27" t="s">
         <v>470</v>
       </c>
-      <c r="N27" s="2" t="s">
+      <c r="O27" t="s">
         <v>67</v>
       </c>
-      <c r="O27" s="2" t="s">
+      <c r="P27" t="s">
         <v>471</v>
       </c>
-      <c r="P27" s="2" t="s">
+      <c r="Q27" t="s">
         <v>472</v>
       </c>
-      <c r="Q27" s="2" t="s">
+      <c r="R27" t="s">
         <v>82</v>
       </c>
-      <c r="R27" s="2" t="s">
+      <c r="S27" t="s">
         <v>473</v>
       </c>
-      <c r="S27" s="2" t="s">
+      <c r="T27" t="s">
         <v>279</v>
       </c>
-      <c r="T27" s="2" t="s">
+      <c r="U27" t="s">
         <v>474</v>
       </c>
-      <c r="U27" s="2" t="s">
+      <c r="V27" t="s">
         <v>475</v>
       </c>
-      <c r="V27" s="2" t="s">
+      <c r="W27" t="s">
         <v>138</v>
       </c>
-      <c r="W27" s="2" t="s">
+      <c r="X27" t="s">
         <v>139</v>
       </c>
-      <c r="X27" s="2" t="s">
+      <c r="Y27" t="s">
         <v>208</v>
       </c>
-      <c r="Y27" s="2" t="s">
+      <c r="Z27" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="28" spans="1:25">
+    <row r="28" spans="1:26">
       <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" t="s">
         <v>477</v>
       </c>
-      <c r="C28">
+      <c r="C28" t="s">
+        <v>575</v>
+      </c>
+      <c r="D28">
         <v>82</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="E28" t="s">
         <v>142</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="F28" t="s">
         <v>478</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="G28" t="s">
         <v>479</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="H28" t="s">
         <v>480</v>
       </c>
-      <c r="H28" s="2" t="s">
+      <c r="I28" t="s">
         <v>213</v>
       </c>
-      <c r="I28" s="2" t="s">
+      <c r="J28" t="s">
         <v>481</v>
       </c>
-      <c r="J28" s="2" t="s">
+      <c r="K28" t="s">
         <v>482</v>
       </c>
-      <c r="K28" s="2" t="s">
+      <c r="L28" t="s">
         <v>483</v>
       </c>
-      <c r="L28" s="2" t="s">
+      <c r="M28" t="s">
         <v>274</v>
       </c>
-      <c r="M28" s="2" t="s">
+      <c r="N28" t="s">
         <v>484</v>
       </c>
-      <c r="N28" s="2" t="s">
+      <c r="O28" t="s">
         <v>310</v>
       </c>
-      <c r="O28" s="2" t="s">
+      <c r="P28" t="s">
         <v>485</v>
       </c>
-      <c r="P28" s="2" t="s">
+      <c r="Q28" t="s">
         <v>460</v>
       </c>
-      <c r="Q28" s="2" t="s">
+      <c r="R28" t="s">
         <v>486</v>
       </c>
-      <c r="R28" s="2" t="s">
+      <c r="S28" t="s">
         <v>487</v>
       </c>
-      <c r="S28" s="2" t="s">
+      <c r="T28" t="s">
         <v>343</v>
       </c>
-      <c r="T28" s="2" t="s">
+      <c r="U28" t="s">
         <v>109</v>
       </c>
-      <c r="U28" s="2" t="s">
+      <c r="V28" t="s">
         <v>488</v>
       </c>
-      <c r="V28" s="2" t="s">
+      <c r="W28" t="s">
         <v>329</v>
       </c>
-      <c r="W28" s="2" t="s">
+      <c r="X28" t="s">
         <v>184</v>
       </c>
-      <c r="X28" s="2" t="s">
+      <c r="Y28" t="s">
         <v>489</v>
       </c>
-      <c r="Y28" s="2" t="s">
+      <c r="Z28" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="29" spans="1:25">
+    <row r="29" spans="1:26">
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" t="s">
         <v>491</v>
       </c>
-      <c r="C29">
+      <c r="C29" t="s">
+        <v>576</v>
+      </c>
+      <c r="D29">
         <v>82</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="E29" t="s">
         <v>57</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="F29" t="s">
         <v>125</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="G29" t="s">
         <v>492</v>
       </c>
-      <c r="G29" s="2" t="s">
+      <c r="H29" t="s">
         <v>493</v>
       </c>
-      <c r="H29" s="2" t="s">
+      <c r="I29" t="s">
         <v>203</v>
       </c>
-      <c r="I29" s="2" t="s">
+      <c r="J29" t="s">
         <v>473</v>
       </c>
-      <c r="J29" s="2" t="s">
+      <c r="K29" t="s">
         <v>494</v>
       </c>
-      <c r="K29" s="2" t="s">
+      <c r="L29" t="s">
         <v>495</v>
       </c>
-      <c r="L29" s="2" t="s">
+      <c r="M29" t="s">
         <v>496</v>
       </c>
-      <c r="M29" s="2" t="s">
+      <c r="N29" t="s">
         <v>497</v>
       </c>
-      <c r="N29" s="2" t="s">
+      <c r="O29" t="s">
         <v>498</v>
       </c>
-      <c r="O29" s="2" t="s">
+      <c r="P29" t="s">
         <v>499</v>
       </c>
-      <c r="P29" s="2" t="s">
+      <c r="Q29" t="s">
         <v>500</v>
       </c>
-      <c r="Q29" s="2" t="s">
+      <c r="R29" t="s">
         <v>210</v>
       </c>
-      <c r="R29" s="2" t="s">
+      <c r="S29" t="s">
         <v>85</v>
       </c>
-      <c r="S29" s="2" t="s">
+      <c r="T29" t="s">
         <v>451</v>
       </c>
-      <c r="T29" s="2" t="s">
+      <c r="U29" t="s">
         <v>501</v>
       </c>
-      <c r="U29" s="2" t="s">
+      <c r="V29" t="s">
         <v>368</v>
       </c>
-      <c r="V29" s="2" t="s">
+      <c r="W29" t="s">
         <v>502</v>
       </c>
-      <c r="W29" s="2" t="s">
+      <c r="X29" t="s">
         <v>503</v>
       </c>
-      <c r="X29" s="2" t="s">
+      <c r="Y29" t="s">
         <v>474</v>
       </c>
-      <c r="Y29" s="2" t="s">
+      <c r="Z29" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="30" spans="1:25">
+    <row r="30" spans="1:26">
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" t="s">
         <v>505</v>
       </c>
-      <c r="C30">
+      <c r="C30" t="s">
+        <v>577</v>
+      </c>
+      <c r="D30">
         <v>82</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="E30" t="s">
         <v>57</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="F30" t="s">
         <v>506</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="G30" t="s">
         <v>162</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="H30" t="s">
         <v>507</v>
       </c>
-      <c r="H30" s="2" t="s">
+      <c r="I30" t="s">
         <v>304</v>
       </c>
-      <c r="I30" s="2" t="s">
+      <c r="J30" t="s">
         <v>467</v>
       </c>
-      <c r="J30" s="2" t="s">
+      <c r="K30" t="s">
         <v>508</v>
       </c>
-      <c r="K30" s="2" t="s">
+      <c r="L30" t="s">
         <v>509</v>
       </c>
-      <c r="L30" s="2" t="s">
+      <c r="M30" t="s">
         <v>510</v>
       </c>
-      <c r="M30" s="2" t="s">
+      <c r="N30" t="s">
         <v>511</v>
       </c>
-      <c r="N30" s="2" t="s">
+      <c r="O30" t="s">
         <v>436</v>
       </c>
-      <c r="O30" s="2" t="s">
+      <c r="P30" t="s">
         <v>415</v>
       </c>
-      <c r="P30" s="2" t="s">
+      <c r="Q30" t="s">
         <v>512</v>
       </c>
-      <c r="Q30" s="2" t="s">
+      <c r="R30" t="s">
         <v>438</v>
       </c>
-      <c r="R30" s="2" t="s">
+      <c r="S30" t="s">
         <v>513</v>
       </c>
-      <c r="S30" s="2" t="s">
+      <c r="T30" t="s">
         <v>514</v>
       </c>
-      <c r="T30" s="2" t="s">
+      <c r="U30" t="s">
         <v>344</v>
       </c>
-      <c r="U30" s="2" t="s">
+      <c r="V30" t="s">
         <v>515</v>
       </c>
-      <c r="V30" s="2" t="s">
+      <c r="W30" t="s">
         <v>329</v>
       </c>
-      <c r="W30" s="2" t="s">
+      <c r="X30" t="s">
         <v>184</v>
       </c>
-      <c r="X30" s="2" t="s">
+      <c r="Y30" t="s">
         <v>415</v>
       </c>
-      <c r="Y30" s="2" t="s">
+      <c r="Z30" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="31" spans="1:25">
+    <row r="31" spans="1:26">
       <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" t="s">
         <v>517</v>
       </c>
-      <c r="C31">
+      <c r="C31" t="s">
+        <v>587</v>
+      </c>
+      <c r="D31">
         <v>82</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="E31" t="s">
         <v>199</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="F31" t="s">
         <v>506</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="G31" t="s">
         <v>518</v>
       </c>
-      <c r="G31" s="2" t="s">
+      <c r="H31" t="s">
         <v>519</v>
       </c>
-      <c r="H31" s="2" t="s">
+      <c r="I31" t="s">
         <v>520</v>
       </c>
-      <c r="I31" s="2" t="s">
+      <c r="J31" t="s">
         <v>444</v>
       </c>
-      <c r="J31" s="2" t="s">
+      <c r="K31" t="s">
         <v>521</v>
       </c>
-      <c r="K31" s="2" t="s">
+      <c r="L31" t="s">
         <v>320</v>
       </c>
-      <c r="L31" s="2" t="s">
+      <c r="M31" t="s">
         <v>522</v>
       </c>
-      <c r="M31" s="2" t="s">
+      <c r="N31" t="s">
         <v>511</v>
       </c>
-      <c r="N31" s="2" t="s">
+      <c r="O31" t="s">
         <v>523</v>
       </c>
-      <c r="O31" s="2" t="s">
+      <c r="P31" t="s">
         <v>140</v>
       </c>
-      <c r="P31" s="2" t="s">
+      <c r="Q31" t="s">
         <v>524</v>
       </c>
-      <c r="Q31" s="2" t="s">
+      <c r="R31" t="s">
         <v>486</v>
       </c>
-      <c r="R31" s="2" t="s">
+      <c r="S31" t="s">
         <v>513</v>
       </c>
-      <c r="S31" s="2" t="s">
+      <c r="T31" t="s">
         <v>525</v>
       </c>
-      <c r="T31" s="2" t="s">
+      <c r="U31" t="s">
         <v>526</v>
       </c>
-      <c r="U31" s="2" t="s">
+      <c r="V31" t="s">
         <v>115</v>
       </c>
-      <c r="V31" s="2" t="s">
+      <c r="W31" t="s">
         <v>401</v>
       </c>
-      <c r="W31" s="2" t="s">
+      <c r="X31" t="s">
         <v>195</v>
       </c>
-      <c r="X31" s="2" t="s">
+      <c r="Y31" t="s">
         <v>409</v>
       </c>
-      <c r="Y31" s="2" t="s">
+      <c r="Z31" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="32" spans="1:25">
-      <c r="B32" s="2" t="s">
+    <row r="32" spans="1:26">
+      <c r="B32" t="s">
         <v>528</v>
       </c>
-      <c r="C32">
+      <c r="C32" t="s">
+        <v>578</v>
+      </c>
+      <c r="D32">
         <v>82</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="E32" t="s">
         <v>529</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="F32" t="s">
         <v>181</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="G32" t="s">
         <v>333</v>
       </c>
-      <c r="G32" s="2" t="s">
+      <c r="H32" t="s">
         <v>81</v>
       </c>
-      <c r="H32" s="2" t="s">
+      <c r="I32" t="s">
         <v>530</v>
       </c>
-      <c r="I32" s="2" t="s">
+      <c r="J32" t="s">
         <v>513</v>
       </c>
-      <c r="J32" s="2" t="s">
+      <c r="K32" t="s">
         <v>531</v>
       </c>
-      <c r="K32" s="2" t="s">
+      <c r="L32" t="s">
         <v>532</v>
       </c>
-      <c r="L32" s="2" t="s">
+      <c r="M32" t="s">
         <v>533</v>
       </c>
-      <c r="M32" s="2" t="s">
+      <c r="N32" t="s">
         <v>534</v>
       </c>
-      <c r="N32" s="2" t="s">
+      <c r="O32" t="s">
         <v>535</v>
       </c>
-      <c r="O32" s="2" t="s">
+      <c r="P32" t="s">
         <v>474</v>
       </c>
-      <c r="P32" s="2" t="s">
+      <c r="Q32" t="s">
         <v>536</v>
       </c>
-      <c r="Q32" s="2" t="s">
+      <c r="R32" t="s">
         <v>226</v>
       </c>
-      <c r="R32" s="2" t="s">
+      <c r="S32" t="s">
         <v>227</v>
       </c>
-      <c r="S32" s="2" t="s">
+      <c r="T32" t="s">
         <v>537</v>
       </c>
-      <c r="T32" s="2" t="s">
+      <c r="U32" t="s">
         <v>175</v>
       </c>
-      <c r="U32" s="2" t="s">
+      <c r="V32" t="s">
         <v>115</v>
       </c>
-      <c r="V32" s="2" t="s">
+      <c r="W32" t="s">
         <v>386</v>
       </c>
-      <c r="W32" s="2" t="s">
+      <c r="X32" t="s">
         <v>538</v>
       </c>
-      <c r="X32" s="2" t="s">
+      <c r="Y32" t="s">
         <v>363</v>
       </c>
-      <c r="Y32" s="2" t="s">
+      <c r="Z32" t="s">
         <v>539</v>
       </c>
     </row>

</xml_diff>